<commit_message>
Avances en el main
</commit_message>
<xml_diff>
--- a/HDT5.xlsx
+++ b/HDT5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Semestre 3\Estructuras de Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\OneDrive\Documentos\GitHub\SimpyHoja\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AE3D58-D3DB-4FAB-B02F-229E07DB90FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" xr2:uid="{6796A8D8-932F-4C76-A363-4DFE643AAF40}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7550" xr2:uid="{6796A8D8-932F-4C76-A363-4DFE643AAF40}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -120,18 +120,18 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2583,242 +2583,242 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42024120-A6C5-429D-B133-CFA02EF77B81}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="2">
         <v>25</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>19.93</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="2">
         <v>50</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>24.45</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="2">
         <v>100</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>43.11</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>25</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>8.15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="2">
         <v>150</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>33.06</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>50</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>23.96</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="2">
         <v>200</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>34.409999999999997</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>100</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>36.979999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K9" s="3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K9" s="2">
         <v>150</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>36.46</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K10" s="3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K10" s="2">
         <v>200</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>39.29</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="J26" s="4" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="J26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J31" s="5" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K31" s="5"/>
+      <c r="K31" s="3"/>
     </row>
-    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K33" s="2" t="s">
+    <row r="33" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="L33" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K34" s="3">
+    <row r="34" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K34" s="2">
         <v>25</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="2">
         <v>2.64</v>
       </c>
     </row>
-    <row r="35" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K35" s="3">
+    <row r="35" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K35" s="2">
         <v>50</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35" s="2">
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="36" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K36" s="3">
+    <row r="36" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K36" s="2">
         <v>100</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="2">
         <v>1.96</v>
       </c>
     </row>
-    <row r="37" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K37" s="3">
+    <row r="37" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K37" s="2">
         <v>150</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37" s="2">
         <v>1.64</v>
       </c>
     </row>
-    <row r="38" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K38" s="3">
+    <row r="38" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K38" s="2">
         <v>200</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="2">
         <v>39.29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J31:K31"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A25:E28"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="J26:N29"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>